<commit_message>
Add latest code updates
</commit_message>
<xml_diff>
--- a/test-data/Base_Test_Invoice.xlsx
+++ b/test-data/Base_Test_Invoice.xlsx
@@ -475,10 +475,10 @@
         <v>CH1</v>
       </c>
       <c r="H2">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" t="str">
         <v>Setup Fee</v>
@@ -493,10 +493,10 @@
         <v>Americas</v>
       </c>
       <c r="N2" t="str">
-        <v>2025-01-01</v>
+        <v>2025-02-15</v>
       </c>
       <c r="O2" t="str">
-        <v>2025-01-01</v>
+        <v>2025-02-15</v>
       </c>
       <c r="P2">
         <v>3</v>
@@ -528,7 +528,7 @@
         <v>12</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J3" t="str">
         <v>Test Service Monthly</v>
@@ -543,13 +543,13 @@
         <v>Americas</v>
       </c>
       <c r="N3" t="str">
-        <v>2025-01-01</v>
+        <v>2025-04-01</v>
       </c>
       <c r="O3" t="str">
-        <v>2025-01-01</v>
+        <v>2025-04-01</v>
       </c>
       <c r="P3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -575,7 +575,7 @@
         <v>DA2</v>
       </c>
       <c r="H4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -593,13 +593,13 @@
         <v>Americas</v>
       </c>
       <c r="N4" t="str">
-        <v>2025-01-01</v>
+        <v>2025-05-10</v>
       </c>
       <c r="O4" t="str">
-        <v>2025-01-01</v>
+        <v>2025-05-10</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -628,7 +628,7 @@
         <v>12</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J5" t="str">
         <v>Test Service Monthly</v>
@@ -643,13 +643,13 @@
         <v>Americas</v>
       </c>
       <c r="N5" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O5" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -675,10 +675,10 @@
         <v>DA1</v>
       </c>
       <c r="H6">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J6" t="str">
         <v>Setup Fee</v>
@@ -693,10 +693,10 @@
         <v>Americas</v>
       </c>
       <c r="N6" t="str">
-        <v>2025-01-01</v>
+        <v>2025-08-01</v>
       </c>
       <c r="O6" t="str">
-        <v>2025-01-01</v>
+        <v>2025-08-01</v>
       </c>
       <c r="P6">
         <v>3</v>
@@ -743,13 +743,13 @@
         <v>Americas</v>
       </c>
       <c r="N7" t="str">
-        <v>2025-01-01</v>
+        <v>2025-09-15</v>
       </c>
       <c r="O7" t="str">
-        <v>2025-01-01</v>
+        <v>2025-09-15</v>
       </c>
       <c r="P7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -775,10 +775,10 @@
         <v>AM2</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J8" t="str">
         <v>Setup Fee</v>
@@ -793,13 +793,13 @@
         <v>Americas</v>
       </c>
       <c r="N8" t="str">
-        <v>2025-01-01</v>
+        <v>2025-11-01</v>
       </c>
       <c r="O8" t="str">
-        <v>2025-01-01</v>
+        <v>2025-11-01</v>
       </c>
       <c r="P8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -828,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J9" t="str">
         <v>Test Service Monthly</v>
@@ -849,7 +849,7 @@
         <v>2025-01-01</v>
       </c>
       <c r="P9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -875,7 +875,7 @@
         <v>CH2</v>
       </c>
       <c r="H10">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I10">
         <v>5</v>
@@ -893,10 +893,10 @@
         <v>Americas</v>
       </c>
       <c r="N10" t="str">
-        <v>2025-01-01</v>
+        <v>2025-02-15</v>
       </c>
       <c r="O10" t="str">
-        <v>2025-01-01</v>
+        <v>2025-02-15</v>
       </c>
       <c r="P10">
         <v>3</v>
@@ -928,7 +928,7 @@
         <v>12</v>
       </c>
       <c r="I11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J11" t="str">
         <v>Test Service Monthly</v>
@@ -943,13 +943,13 @@
         <v>Americas</v>
       </c>
       <c r="N11" t="str">
-        <v>2025-01-01</v>
+        <v>2025-04-01</v>
       </c>
       <c r="O11" t="str">
-        <v>2025-01-01</v>
+        <v>2025-04-01</v>
       </c>
       <c r="P11">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -975,10 +975,10 @@
         <v>CH1</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J12" t="str">
         <v>Setup Fee</v>
@@ -993,13 +993,13 @@
         <v>Americas</v>
       </c>
       <c r="N12" t="str">
-        <v>2025-01-01</v>
+        <v>2025-05-10</v>
       </c>
       <c r="O12" t="str">
-        <v>2025-01-01</v>
+        <v>2025-05-10</v>
       </c>
       <c r="P12">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -1043,13 +1043,13 @@
         <v>Americas</v>
       </c>
       <c r="N13" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O13" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1075,10 +1075,10 @@
         <v>DA2</v>
       </c>
       <c r="H14">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J14" t="str">
         <v>Setup Fee</v>
@@ -1093,10 +1093,10 @@
         <v>Americas</v>
       </c>
       <c r="N14" t="str">
-        <v>2025-01-01</v>
+        <v>2025-08-01</v>
       </c>
       <c r="O14" t="str">
-        <v>2025-01-01</v>
+        <v>2025-08-01</v>
       </c>
       <c r="P14">
         <v>3</v>
@@ -1128,7 +1128,7 @@
         <v>12</v>
       </c>
       <c r="I15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J15" t="str">
         <v>Test Service Monthly</v>
@@ -1143,13 +1143,13 @@
         <v>Americas</v>
       </c>
       <c r="N15" t="str">
-        <v>2025-01-01</v>
+        <v>2025-09-15</v>
       </c>
       <c r="O15" t="str">
-        <v>2025-01-01</v>
+        <v>2025-09-15</v>
       </c>
       <c r="P15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -1175,7 +1175,7 @@
         <v>DA1</v>
       </c>
       <c r="H16">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I16">
         <v>5</v>
@@ -1193,13 +1193,13 @@
         <v>Americas</v>
       </c>
       <c r="N16" t="str">
-        <v>2025-01-01</v>
+        <v>2025-11-01</v>
       </c>
       <c r="O16" t="str">
-        <v>2025-01-01</v>
+        <v>2025-11-01</v>
       </c>
       <c r="P16">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -1228,7 +1228,7 @@
         <v>12</v>
       </c>
       <c r="I17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J17" t="str">
         <v>Test Service Monthly</v>
@@ -1249,7 +1249,7 @@
         <v>2025-01-01</v>
       </c>
       <c r="P17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1275,10 +1275,10 @@
         <v>AM2</v>
       </c>
       <c r="H18">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J18" t="str">
         <v>Setup Fee</v>
@@ -1293,10 +1293,10 @@
         <v>Americas</v>
       </c>
       <c r="N18" t="str">
-        <v>2025-01-01</v>
+        <v>2025-02-15</v>
       </c>
       <c r="O18" t="str">
-        <v>2025-01-01</v>
+        <v>2025-02-15</v>
       </c>
       <c r="P18">
         <v>3</v>
@@ -1343,13 +1343,13 @@
         <v>Americas</v>
       </c>
       <c r="N19" t="str">
-        <v>2025-01-01</v>
+        <v>2025-04-01</v>
       </c>
       <c r="O19" t="str">
-        <v>2025-01-01</v>
+        <v>2025-04-01</v>
       </c>
       <c r="P19">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -1375,10 +1375,10 @@
         <v>CH2</v>
       </c>
       <c r="H20">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="I20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J20" t="str">
         <v>Setup Fee</v>
@@ -1393,13 +1393,13 @@
         <v>Americas</v>
       </c>
       <c r="N20" t="str">
-        <v>2025-01-01</v>
+        <v>2025-05-10</v>
       </c>
       <c r="O20" t="str">
-        <v>2025-01-01</v>
+        <v>2025-05-10</v>
       </c>
       <c r="P20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -1428,7 +1428,7 @@
         <v>12</v>
       </c>
       <c r="I21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J21" t="str">
         <v>Test Service Monthly</v>
@@ -1443,13 +1443,13 @@
         <v>Americas</v>
       </c>
       <c r="N21" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O21" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -2057,7 +2057,7 @@
         <v>INV-33</v>
       </c>
       <c r="B34" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2093,10 +2093,10 @@
         <v>Americas</v>
       </c>
       <c r="N34" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O34" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P34" t="str">
         <v/>
@@ -2107,7 +2107,7 @@
         <v>INV-34</v>
       </c>
       <c r="B35" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2143,10 +2143,10 @@
         <v>Americas</v>
       </c>
       <c r="N35" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O35" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P35" t="str">
         <v/>
@@ -2157,7 +2157,7 @@
         <v>INV-35</v>
       </c>
       <c r="B36" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2193,10 +2193,10 @@
         <v>Americas</v>
       </c>
       <c r="N36" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O36" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P36" t="str">
         <v/>
@@ -2207,7 +2207,7 @@
         <v>INV-36</v>
       </c>
       <c r="B37" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2243,10 +2243,10 @@
         <v>Americas</v>
       </c>
       <c r="N37" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O37" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P37" t="str">
         <v/>
@@ -2257,7 +2257,7 @@
         <v>INV-37</v>
       </c>
       <c r="B38" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2293,10 +2293,10 @@
         <v>Americas</v>
       </c>
       <c r="N38" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O38" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P38" t="str">
         <v/>
@@ -2307,7 +2307,7 @@
         <v>INV-38</v>
       </c>
       <c r="B39" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2343,10 +2343,10 @@
         <v>Americas</v>
       </c>
       <c r="N39" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O39" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P39" t="str">
         <v/>
@@ -2357,7 +2357,7 @@
         <v>INV-39</v>
       </c>
       <c r="B40" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2393,10 +2393,10 @@
         <v>Americas</v>
       </c>
       <c r="N40" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O40" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P40" t="str">
         <v/>
@@ -2407,7 +2407,7 @@
         <v>INV-40</v>
       </c>
       <c r="B41" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2443,10 +2443,10 @@
         <v>Americas</v>
       </c>
       <c r="N41" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O41" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P41" t="str">
         <v/>
@@ -2457,7 +2457,7 @@
         <v>INV-41</v>
       </c>
       <c r="B42" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2493,10 +2493,10 @@
         <v>Americas</v>
       </c>
       <c r="N42" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O42" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P42" t="str">
         <v/>
@@ -2507,7 +2507,7 @@
         <v>INV-42</v>
       </c>
       <c r="B43" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2543,10 +2543,10 @@
         <v>Americas</v>
       </c>
       <c r="N43" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O43" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P43" t="str">
         <v/>
@@ -2557,7 +2557,7 @@
         <v>INV-43</v>
       </c>
       <c r="B44" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2593,10 +2593,10 @@
         <v>Americas</v>
       </c>
       <c r="N44" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O44" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P44" t="str">
         <v/>
@@ -2607,7 +2607,7 @@
         <v>INV-44</v>
       </c>
       <c r="B45" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2643,10 +2643,10 @@
         <v>Americas</v>
       </c>
       <c r="N45" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O45" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P45" t="str">
         <v/>
@@ -2657,7 +2657,7 @@
         <v>INV-45</v>
       </c>
       <c r="B46" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2693,10 +2693,10 @@
         <v>Americas</v>
       </c>
       <c r="N46" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O46" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P46" t="str">
         <v/>
@@ -2707,7 +2707,7 @@
         <v>INV-46</v>
       </c>
       <c r="B47" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2743,10 +2743,10 @@
         <v>Americas</v>
       </c>
       <c r="N47" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O47" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P47" t="str">
         <v/>
@@ -2757,7 +2757,7 @@
         <v>INV-47</v>
       </c>
       <c r="B48" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2793,10 +2793,10 @@
         <v>Americas</v>
       </c>
       <c r="N48" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O48" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P48" t="str">
         <v/>
@@ -2807,7 +2807,7 @@
         <v>INV-48</v>
       </c>
       <c r="B49" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2843,10 +2843,10 @@
         <v>Americas</v>
       </c>
       <c r="N49" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O49" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P49" t="str">
         <v/>
@@ -2857,7 +2857,7 @@
         <v>INV-49</v>
       </c>
       <c r="B50" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2893,10 +2893,10 @@
         <v>Americas</v>
       </c>
       <c r="N50" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O50" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P50" t="str">
         <v/>
@@ -2907,7 +2907,7 @@
         <v>INV-50</v>
       </c>
       <c r="B51" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2943,10 +2943,10 @@
         <v>Americas</v>
       </c>
       <c r="N51" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O51" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P51" t="str">
         <v/>
@@ -2957,7 +2957,7 @@
         <v>INV-51</v>
       </c>
       <c r="B52" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2993,10 +2993,10 @@
         <v>Americas</v>
       </c>
       <c r="N52" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O52" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P52" t="str">
         <v/>
@@ -3007,7 +3007,7 @@
         <v>INV-52</v>
       </c>
       <c r="B53" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3057,7 +3057,7 @@
         <v>INV-53</v>
       </c>
       <c r="B54" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3107,7 +3107,7 @@
         <v>INV-54</v>
       </c>
       <c r="B55" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3157,7 +3157,7 @@
         <v>INV-55</v>
       </c>
       <c r="B56" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3207,7 +3207,7 @@
         <v>INV-56</v>
       </c>
       <c r="B57" t="str">
-        <v>2025-01-15</v>
+        <v>2025-06-15</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3243,10 +3243,10 @@
         <v>Americas</v>
       </c>
       <c r="N57" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="O57" t="str">
-        <v>2025-01-01</v>
+        <v>2025-06-01</v>
       </c>
       <c r="P57" t="str">
         <v/>

</xml_diff>